<commit_message>
14/01/2020 trendyol and morhipo changed
</commit_message>
<xml_diff>
--- a/Genbot.UI/Assets/Upload/turan/deneme.xlsx
+++ b/Genbot.UI/Assets/Upload/turan/deneme.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbalt\Desktop\Günerler Excelss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbalt\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2859CDAE-ACE3-4382-AC69-119B76528595}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5D60E2-58CE-4257-8435-D6F13C32A463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -36,32 +36,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF6B6F82"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color rgb="FF333333"/>
-      <name val="Source_sans_proregular"/>
+      <charset val="162"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,20 +59,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{910D6A48-D074-4BAB-8558-55297D9B7A96}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -364,75 +345,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A20"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" ht="16.5">
-      <c r="A2" s="3">
-        <v>3605532209067</v>
+    <row r="2" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>8699490222850</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="18.75">
-      <c r="A4" s="4"/>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="1"/>
+    <row r="3" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>8699490221419</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>